<commit_message>
Corrigiendo permisos del Regente
</commit_message>
<xml_diff>
--- a/Guia 5/permisos.xlsx
+++ b/Guia 5/permisos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\menji\OneDrive - Universidad de Sonsonate\CICLO V - USO\CICLO V - TAREAS\TAREAS - LAB. BASE DE DATOS I\LaboratorioBDI\GUIA05\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D97E815D-0FEF-4E70-9545-6DB90AB24A89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD38377F-8F0B-459B-9BF7-6094114F99DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{4454E307-B2E1-4A50-BD93-81C4DDD0B701}"/>
   </bookViews>
@@ -59,9 +59,6 @@
     <t>Regente</t>
   </si>
   <si>
-    <t>CRUD(medicamentos,formulas,sucursales)</t>
-  </si>
-  <si>
     <t>regente@gmail.com</t>
   </si>
   <si>
@@ -117,6 +114,9 @@
   </si>
   <si>
     <t>CRUD(empleados,cargos,direcciones)    LECTURA(distritos,municipios,departamentos)</t>
+  </si>
+  <si>
+    <t>CRUD(medicamentos,sucursales)</t>
   </si>
 </sst>
 </file>
@@ -560,7 +560,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -597,76 +597,76 @@
         <v>6</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>7</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="C4" s="4" t="s">
         <v>10</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="C5" s="4" t="s">
         <v>13</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="C6" s="4" t="s">
         <v>16</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="C7" s="4" t="s">
         <v>19</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>21</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>23</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>